<commit_message>
Added other test logins
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\Software-Engineering-Banking-Project-Phase-2-UI\Software-Engineering-Banking-Project\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD6673B-8327-4CDB-A09D-A578F666183F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CEB7DD-9BBF-450F-BCFE-CD89E37DD7E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>cmoticska</t>
   </si>
@@ -50,15 +50,6 @@
     <t>214dc12efd3c0819ae541ffa1f18cf5642a5118d9aa82e570957d46393c59d24</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -72,6 +63,33 @@
   </si>
   <si>
     <t>banana</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Edwards</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Columbo</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>jedwards</t>
+  </si>
+  <si>
+    <t>mcolumbo</t>
+  </si>
+  <si>
+    <t>arivera</t>
   </si>
 </sst>
 </file>
@@ -428,7 +446,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,42 +482,60 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the password for cmoticska login
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\Software-Engineering-Banking-Project-Phase-2-UI\Software-Engineering-Banking-Project\src\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CEB7DD-9BBF-450F-BCFE-CD89E37DD7E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBB25D4-5931-4A23-959C-043E0D22C5E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="4230" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Moticska</t>
   </si>
   <si>
-    <t>214dc12efd3c0819ae541ffa1f18cf5642a5118d9aa82e570957d46393c59d24</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>arivera</t>
+  </si>
+  <si>
+    <t>5e884898da28047151d0e56f8dc6292773603d0d6aabbdd62a11ef721d1542d8</t>
   </si>
 </sst>
 </file>
@@ -125,10 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +447,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,66 +477,66 @@
       <c r="G1" s="2">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added passwords for every account
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FB78A9-3056-4283-95A0-0B7BF9FA6902}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E7A879-ECED-479D-BD8A-8568CE71AE07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="7965" yWindow="3600" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>cmoticska</t>
   </si>
@@ -92,7 +92,22 @@
     <t>b14d501a594442a01c6859541bcb3e8164d183d32937b851835442f69d5c94e</t>
   </si>
   <si>
-    <t>9323dd6786ebcbf3ac87357cc78ba1abfda6cf5e55cd01097b90d4a286cac90e</t>
+    <t>6cf615d5bcaac778352a8f1f3360d23f02f34ec182e259897fd6ce485d7870d4</t>
+  </si>
+  <si>
+    <t>5906ac361a137e2d286465cd6588ebb5ac3f5ae955001100bc41577c3d751764</t>
+  </si>
+  <si>
+    <t>b97873a40f73abedd8d685a7cd5e5f85e4a9cfb83eac26886640a0813850122b</t>
+  </si>
+  <si>
+    <t>8b2c86ea9cf2ea4eb517fd1e06b74f399e7fec0fef92e3b482a6cf2e2b092023</t>
+  </si>
+  <si>
+    <t>598a1a400c1dfdf36974e69d7e1bc98593f2e15015eed8e9b7e47a83b31693d5</t>
+  </si>
+  <si>
+    <t>5860836e8f13fc9837539a597d4086bfc0299e54ad92148d54538b5c3feefb7c</t>
   </si>
 </sst>
 </file>
@@ -447,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A33469-0456-4818-B15F-DDC4B5E86F1B}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +493,7 @@
         <v>44440</v>
       </c>
       <c r="G1" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
@@ -494,6 +509,9 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
@@ -508,6 +526,12 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -519,28 +543,55 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="H9" t="s">
-        <v>18</v>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added top row to show parameters
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E7A879-ECED-479D-BD8A-8568CE71AE07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348BC16-E42B-496B-9E93-49904AD8F3D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="3600" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
-    <sheet name="RegisterList" sheetId="3" r:id="rId2"/>
-    <sheet name="DeleteList" sheetId="4" r:id="rId3"/>
+    <sheet name="RequestList" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>cmoticska</t>
   </si>
@@ -108,6 +107,30 @@
   </si>
   <si>
     <t>5860836e8f13fc9837539a597d4086bfc0299e54ad92148d54538b5c3feefb7c</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>DoB</t>
+  </si>
+  <si>
+    <t>Card #</t>
+  </si>
+  <si>
+    <t>Last Accessed</t>
+  </si>
+  <si>
+    <t>Employee Status</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -462,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A33469-0456-4818-B15F-DDC4B5E86F1B}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,122 +498,148 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>36770</v>
-      </c>
-      <c r="E1" s="2">
-        <v>123456789</v>
-      </c>
-      <c r="F1" s="1">
-        <v>44440</v>
-      </c>
-      <c r="G1" s="2">
-        <v>1</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>36770</v>
+      </c>
+      <c r="E2" s="2">
+        <v>123456789</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44440</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -610,16 +659,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6CD8E6-1E06-46B6-BB61-1C9828CD852B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more for testing
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F348BC16-E42B-496B-9E93-49904AD8F3D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D2E0A-7708-43D7-8D4D-CE47C81488A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>cmoticska</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Chris</t>
   </si>
 </sst>
 </file>
@@ -487,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A33469-0456-4818-B15F-DDC4B5E86F1B}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,12 +654,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F42263E-EB85-4CF0-A25D-7A19F1ADB73B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed how employee status is seen
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5D2E0A-7708-43D7-8D4D-CE47C81488A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5290A7-FE10-4105-B7B3-2B1190CDB141}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>cmoticska</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Chris</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -172,8 +175,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,13 +493,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A33469-0456-4818-B15F-DDC4B5E86F1B}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -538,16 +542,16 @@
       <c r="D2" s="1">
         <v>36770</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>123456789</v>
       </c>
       <c r="F2" s="1">
         <v>44440</v>
       </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -561,8 +565,9 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="E3" s="3"/>
+      <c r="G3" t="s">
+        <v>33</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -578,8 +583,9 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="E4" s="3"/>
+      <c r="G4" t="s">
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -595,8 +601,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="G5">
-        <v>1</v>
+      <c r="E5" s="3"/>
+      <c r="G5" t="s">
+        <v>33</v>
       </c>
       <c r="H5" t="s">
         <v>19</v>
@@ -606,8 +613,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>0</v>
+      <c r="E6" s="3"/>
+      <c r="G6" t="s">
+        <v>4</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -617,8 +625,9 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="G7">
-        <v>0</v>
+      <c r="E7" s="3"/>
+      <c r="G7" t="s">
+        <v>4</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -628,8 +637,9 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="E8" s="3"/>
+      <c r="G8" t="s">
+        <v>4</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -639,8 +649,9 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="G9">
-        <v>0</v>
+      <c r="E9" s="3"/>
+      <c r="G9" t="s">
+        <v>4</v>
       </c>
       <c r="H9" t="s">
         <v>23</v>
@@ -656,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F42263E-EB85-4CF0-A25D-7A19F1ADB73B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added cards to every user
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549B56FF-07B1-4AD1-B1BB-6ED61F6A52F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC94F7C5-D879-4D98-AFB5-E92C842DE2CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="3375" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="3555" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,9 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>100000001</v>
+      </c>
       <c r="F3" t="s">
         <v>32</v>
       </c>
@@ -589,7 +591,9 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>100000002</v>
+      </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>
@@ -607,7 +611,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>100000003</v>
+      </c>
       <c r="F5" t="s">
         <v>32</v>
       </c>
@@ -625,7 +631,9 @@
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>100000004</v>
+      </c>
       <c r="F6" t="s">
         <v>4</v>
       </c>
@@ -643,7 +651,9 @@
       <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>100000005</v>
+      </c>
       <c r="F7" t="s">
         <v>4</v>
       </c>
@@ -661,7 +671,9 @@
       <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>100000006</v>
+      </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
@@ -679,7 +691,9 @@
       <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>100000007</v>
+      </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added transact history for all current users
</commit_message>
<xml_diff>
--- a/bin/Database/Database.xlsx
+++ b/bin/Database/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\BankingProjectPhase2UI\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC94F7C5-D879-4D98-AFB5-E92C842DE2CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E13DFC-7B98-4E5C-8508-22ED4651D282}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="4365" windowWidth="21600" windowHeight="11835" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
+    <workbookView xWindow="6000" yWindow="3450" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{E1FE871D-B3B0-4578-A128-876B4185847E}"/>
   </bookViews>
   <sheets>
     <sheet name="UserList" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A33469-0456-4818-B15F-DDC4B5E86F1B}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -711,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F42263E-EB85-4CF0-A25D-7A19F1ADB73B}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>